<commit_message>
Recent ARTnet RADAR Work Commit
</commit_message>
<xml_diff>
--- a/Analysis/Chicago YMSM Model/Chicago NetParams Validation.xlsx
+++ b/Analysis/Chicago YMSM Model/Chicago NetParams Validation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\EpiModel Lab\ARTnet RADAR Mean Degree Comparison\ARTnet-RADAR\Analysis\ARTnet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\EpiModel Lab\ARTnet RADAR Mean Degree Comparison\ARTnet-RADAR\Analysis\Chicago YMSM Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C89D37B3-9A24-452B-A814-64B436675420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADA9490-35F5-4475-8AFB-47FF56550A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,31 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{DD22C88E-E335-42A9-B38E-A9942F8C7A43}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Connor Van Meter:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-out$casl$nm.age.grp_diffF</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R26" authorId="0" shapeId="0" xr:uid="{AACBC661-CF0E-49E2-86EA-B2D111E75D28}">
+    <comment ref="R25" authorId="0" shapeId="0" xr:uid="{AACBC661-CF0E-49E2-86EA-B2D111E75D28}">
       <text>
         <r>
           <rPr>
@@ -472,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R30" authorId="0" shapeId="0" xr:uid="{95091133-B49A-4C79-8444-DD2E2DC78C02}">
+    <comment ref="R29" authorId="0" shapeId="0" xr:uid="{95091133-B49A-4C79-8444-DD2E2DC78C02}">
       <text>
         <r>
           <rPr>
@@ -496,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R32" authorId="0" shapeId="0" xr:uid="{A4E920F7-9105-4EC9-9B1B-66A069D171A6}">
+    <comment ref="R31" authorId="0" shapeId="0" xr:uid="{A4E920F7-9105-4EC9-9B1B-66A069D171A6}">
       <text>
         <r>
           <rPr>
@@ -520,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R39" authorId="0" shapeId="0" xr:uid="{85649896-69D2-446F-B912-EA58E2DFE0E5}">
+    <comment ref="R38" authorId="0" shapeId="0" xr:uid="{85649896-69D2-446F-B912-EA58E2DFE0E5}">
       <text>
         <r>
           <rPr>
@@ -544,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R41" authorId="0" shapeId="0" xr:uid="{08A2BF65-7B01-420C-9C9D-C995F8E7D4A7}">
+    <comment ref="R40" authorId="0" shapeId="0" xr:uid="{08A2BF65-7B01-420C-9C9D-C995F8E7D4A7}">
       <text>
         <r>
           <rPr>
@@ -568,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{55B5EB2D-1E8B-45AC-9C2F-8F4676398ABA}">
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{55B5EB2D-1E8B-45AC-9C2F-8F4676398ABA}">
       <text>
         <r>
           <rPr>
@@ -592,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J47" authorId="0" shapeId="0" xr:uid="{4C4FF74D-816E-48FA-8F9A-249E27DE3923}">
+    <comment ref="J46" authorId="0" shapeId="0" xr:uid="{4C4FF74D-816E-48FA-8F9A-249E27DE3923}">
       <text>
         <r>
           <rPr>
@@ -621,7 +597,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="85">
   <si>
     <t>San Francisco</t>
   </si>
@@ -3310,10 +3286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29583D5-FBDA-9342-8890-DEB7B7EC6DF8}">
-  <dimension ref="A1:X61"/>
+  <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -4666,117 +4642,123 @@
     </row>
     <row r="24" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="39">
-        <v>0.47</v>
-      </c>
-      <c r="C24" s="52">
-        <f>ABS(B24-E24)</f>
-        <v>0.47</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="39"/>
       <c r="E24" s="39"/>
-      <c r="F24" s="52">
-        <f>ABS(E24-G24)</f>
-        <v>0.47</v>
-      </c>
-      <c r="G24" s="39">
-        <v>0.47</v>
-      </c>
-      <c r="H24" s="52">
-        <f>ABS(B24-G24)</f>
-        <v>0</v>
-      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="35"/>
-      <c r="J24" s="39">
-        <v>0.34</v>
-      </c>
-      <c r="K24" s="52">
-        <f>ABS(J24-M24)</f>
-        <v>0.34</v>
-      </c>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
-      <c r="N24" s="52">
-        <f>ABS(M24-O24)</f>
-        <v>0.38</v>
-      </c>
-      <c r="O24" s="30">
-        <v>0.38</v>
-      </c>
-      <c r="P24" s="52">
-        <f>ABS(J24-O24)</f>
-        <v>3.999999999999998E-2</v>
-      </c>
+      <c r="N24" s="35"/>
+      <c r="P24" s="30"/>
       <c r="Q24" s="35"/>
-      <c r="R24" s="39">
-        <v>0.4</v>
-      </c>
-      <c r="S24" s="52">
-        <f>ABS(R24-U24)</f>
-        <v>0.4</v>
-      </c>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
       <c r="T24" s="39"/>
       <c r="U24" s="39"/>
-      <c r="V24" s="52">
-        <f>ABS(U24-W24)</f>
-        <v>0.39</v>
-      </c>
-      <c r="W24" s="30">
-        <v>0.39</v>
-      </c>
-      <c r="X24" s="52">
-        <f>ABS(R24-W24)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
+      <c r="X24" s="30"/>
     </row>
     <row r="25" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
+      <c r="A25" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="39">
+        <v>0.65800360000000002</v>
+      </c>
+      <c r="C25" s="52">
+        <f>ABS(B25-E25)</f>
+        <v>1.1796399999999929E-2</v>
+      </c>
       <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
+      <c r="E25" s="39">
+        <v>0.66979999999999995</v>
+      </c>
+      <c r="F25" s="52">
+        <f>ABS(E25-G25)</f>
+        <v>1.1796399999999929E-2</v>
+      </c>
+      <c r="G25" s="39">
+        <v>0.65800360000000002</v>
+      </c>
+      <c r="H25" s="52">
+        <f>ABS(B25-G25)</f>
+        <v>0</v>
+      </c>
       <c r="I25" s="35"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
+      <c r="J25" s="39">
+        <v>0.50237069999999995</v>
+      </c>
+      <c r="K25" s="52">
+        <f>ABS(J25-M25)</f>
+        <v>6.1126999999999709E-3</v>
+      </c>
       <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="35"/>
-      <c r="P25" s="30"/>
+      <c r="M25" s="39">
+        <v>0.49625799999999998</v>
+      </c>
+      <c r="N25" s="52">
+        <f>ABS(M25-O25)</f>
+        <v>6.1126999999999709E-3</v>
+      </c>
+      <c r="O25" s="39">
+        <v>0.50237069999999995</v>
+      </c>
+      <c r="P25" s="52">
+        <f>ABS(J25-O25)</f>
+        <v>0</v>
+      </c>
       <c r="Q25" s="35"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
+      <c r="R25" s="39">
+        <v>0.45897450000000001</v>
+      </c>
+      <c r="S25" s="52">
+        <f>ABS(R25-U25)</f>
+        <v>1.3974500000000001E-2</v>
+      </c>
       <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-      <c r="X25" s="30"/>
+      <c r="U25" s="39">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="V25" s="52">
+        <f>ABS(U25-W25)</f>
+        <v>1.3974500000000001E-2</v>
+      </c>
+      <c r="W25" s="39">
+        <v>0.45897450000000001</v>
+      </c>
+      <c r="X25" s="52">
+        <f>ABS(R25-W25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="39">
-        <v>0.61</v>
+        <v>0.68790090000000004</v>
       </c>
       <c r="C26" s="52">
         <f>ABS(B26-E26)</f>
-        <v>5.9799999999999964E-2</v>
+        <v>2.2599099999999983E-2</v>
       </c>
       <c r="D26" s="39"/>
       <c r="E26" s="39">
-        <v>0.66979999999999995</v>
+        <v>0.71050000000000002</v>
       </c>
       <c r="F26" s="52">
         <f>ABS(E26-G26)</f>
-        <v>5.9799999999999964E-2</v>
+        <v>2.2599099999999983E-2</v>
       </c>
       <c r="G26" s="39">
-        <v>0.61</v>
+        <v>0.68790090000000004</v>
       </c>
       <c r="H26" s="52">
         <f>ABS(B26-G26)</f>
@@ -4784,540 +4766,495 @@
       </c>
       <c r="I26" s="35"/>
       <c r="J26" s="39">
-        <v>0.43</v>
+        <v>0.5563034</v>
       </c>
       <c r="K26" s="52">
         <f>ABS(J26-M26)</f>
-        <v>6.6257999999999984E-2</v>
+        <v>9.0339999999999865E-4</v>
       </c>
       <c r="L26" s="39"/>
       <c r="M26" s="39">
-        <v>0.49625799999999998</v>
+        <v>0.5554</v>
       </c>
       <c r="N26" s="52">
         <f>ABS(M26-O26)</f>
-        <v>3.6257999999999957E-2</v>
-      </c>
-      <c r="O26" s="30">
-        <v>0.46</v>
+        <v>9.0339999999999865E-4</v>
+      </c>
+      <c r="O26" s="39">
+        <v>0.5563034</v>
       </c>
       <c r="P26" s="52">
         <f>ABS(J26-O26)</f>
-        <v>3.0000000000000027E-2</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="35"/>
       <c r="R26" s="39">
-        <v>0.43</v>
+        <v>0.5745034</v>
       </c>
       <c r="S26" s="52">
         <f>ABS(R26-U26)</f>
-        <v>1.5000000000000013E-2</v>
+        <v>1.5034000000000436E-3</v>
       </c>
       <c r="T26" s="39"/>
       <c r="U26" s="39">
-        <v>0.44500000000000001</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="V26" s="52">
         <f>ABS(U26-W26)</f>
-        <v>2.5000000000000022E-2</v>
-      </c>
-      <c r="W26" s="30">
-        <v>0.42</v>
+        <v>1.5034000000000436E-3</v>
+      </c>
+      <c r="W26" s="39">
+        <v>0.5745034</v>
       </c>
       <c r="X26" s="52">
         <f>ABS(R26-W26)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" s="39">
-        <v>0.51</v>
+        <v>0.71631140000000004</v>
       </c>
       <c r="C27" s="52">
         <f>ABS(B27-E27)</f>
-        <v>0.20050000000000001</v>
+        <v>3.1788599999999945E-2</v>
       </c>
       <c r="D27" s="39"/>
       <c r="E27" s="39">
-        <v>0.71050000000000002</v>
+        <v>0.74809999999999999</v>
       </c>
       <c r="F27" s="52">
         <f>ABS(E27-G27)</f>
-        <v>0.21050000000000002</v>
-      </c>
-      <c r="G27" s="30">
-        <v>0.5</v>
+        <v>3.1788599999999945E-2</v>
+      </c>
+      <c r="G27" s="39">
+        <v>0.71631140000000004</v>
       </c>
       <c r="H27" s="52">
         <f>ABS(B27-G27)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="35"/>
       <c r="J27" s="39">
-        <v>0.36</v>
+        <v>0.60894090000000001</v>
       </c>
       <c r="K27" s="52">
         <f>ABS(J27-M27)</f>
-        <v>0.19540000000000002</v>
+        <v>4.0721000000000229E-3</v>
       </c>
       <c r="L27" s="39"/>
       <c r="M27" s="39">
-        <v>0.5554</v>
+        <v>0.61301300000000003</v>
       </c>
       <c r="N27" s="52">
         <f>ABS(M27-O27)</f>
-        <v>0.15539999999999998</v>
-      </c>
-      <c r="O27" s="30">
-        <v>0.4</v>
+        <v>4.0721000000000229E-3</v>
+      </c>
+      <c r="O27" s="39">
+        <v>0.60894090000000001</v>
       </c>
       <c r="P27" s="52">
         <f>ABS(J27-O27)</f>
-        <v>4.0000000000000036E-2</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="35"/>
       <c r="R27" s="39">
-        <v>0.4</v>
+        <v>0.68243180000000003</v>
       </c>
       <c r="S27" s="52">
         <f>ABS(R27-U27)</f>
-        <v>0.17299999999999993</v>
+        <v>8.5681999999999148E-3</v>
       </c>
       <c r="T27" s="39"/>
       <c r="U27" s="39">
-        <v>0.57299999999999995</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="V27" s="52">
         <f>ABS(U27-W27)</f>
-        <v>0.18299999999999994</v>
-      </c>
-      <c r="W27" s="30">
-        <v>0.39</v>
+        <v>8.5681999999999148E-3</v>
+      </c>
+      <c r="W27" s="39">
+        <v>0.68243180000000003</v>
       </c>
       <c r="X27" s="52">
         <f>ABS(R27-W27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="35"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="X28" s="30"/>
+    </row>
+    <row r="29" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="39">
+        <v>0.51</v>
+      </c>
+      <c r="C29" s="52">
+        <f>ABS(B29-E29)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="39">
+        <v>0.51</v>
+      </c>
+      <c r="F29" s="52">
+        <f>ABS(E29-G29)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="30">
+        <v>0.51</v>
+      </c>
+      <c r="H29" s="52">
+        <f>ABS(B29-G29)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="39">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K29" s="52">
+        <f>ABS(J29-M29)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N29" s="52">
+        <f>ABS(M29-O29)</f>
+        <v>1.9999999999999907E-2</v>
+      </c>
+      <c r="O29" s="39">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P29" s="52">
+        <f>ABS(J29-O29)</f>
+        <v>1.9999999999999907E-2</v>
+      </c>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="39">
+        <v>0.66</v>
+      </c>
+      <c r="S29" s="52">
+        <f>ABS(R29-U29)</f>
         <v>1.0000000000000009E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="39">
-        <v>0.4</v>
-      </c>
-      <c r="C28" s="52">
-        <f>ABS(B28-E28)</f>
-        <v>0.34809999999999997</v>
-      </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39">
-        <v>0.74809999999999999</v>
-      </c>
-      <c r="F28" s="52">
-        <f>ABS(E28-G28)</f>
-        <v>0.34809999999999997</v>
-      </c>
-      <c r="G28" s="30">
-        <v>0.4</v>
-      </c>
-      <c r="H28" s="52">
-        <f>ABS(B28-G28)</f>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39">
+        <v>0.65</v>
+      </c>
+      <c r="V29" s="52">
+        <f>ABS(U29-W29)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="35"/>
-      <c r="J28" s="39">
-        <v>0.31</v>
-      </c>
-      <c r="K28" s="52">
-        <f>ABS(J28-M28)</f>
-        <v>0.30301300000000003</v>
-      </c>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39">
-        <v>0.61301300000000003</v>
-      </c>
-      <c r="N28" s="52">
-        <f>ABS(M28-O28)</f>
-        <v>0.27301300000000001</v>
-      </c>
-      <c r="O28" s="30">
-        <v>0.34</v>
-      </c>
-      <c r="P28" s="52">
-        <f>ABS(J28-O28)</f>
-        <v>3.0000000000000027E-2</v>
-      </c>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="39">
-        <v>0.38</v>
-      </c>
-      <c r="S28" s="52">
-        <f>ABS(R28-U28)</f>
-        <v>0.31099999999999994</v>
-      </c>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="V28" s="52">
-        <f>ABS(U28-W28)</f>
-        <v>0.32099999999999995</v>
-      </c>
-      <c r="W28" s="30">
-        <v>0.37</v>
-      </c>
-      <c r="X28" s="52">
-        <f>ABS(R28-W28)</f>
+      <c r="W29" s="30">
+        <v>0.65</v>
+      </c>
+      <c r="X29" s="52">
+        <f>ABS(R29-W29)</f>
         <v>1.0000000000000009E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="35"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="X29" s="30"/>
     </row>
     <row r="30" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="39">
-        <v>0.51</v>
-      </c>
-      <c r="C30" s="52">
-        <f>ABS(B30-E30)</f>
+        <v>53</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="35"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="39"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="39"/>
+      <c r="X30" s="30"/>
+    </row>
+    <row r="31" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="39">
+        <v>0.23</v>
+      </c>
+      <c r="C31" s="52">
+        <f>ABS(B31-E31)</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D31" s="59"/>
+      <c r="E31" s="39">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="F31" s="52">
+        <f>ABS(E31-G31)</f>
+        <v>4.4000000000000011E-2</v>
+      </c>
+      <c r="G31" s="30">
+        <v>0.27</v>
+      </c>
+      <c r="H31" s="52">
+        <f>ABS(B31-G31)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="I31" s="35"/>
+      <c r="J31" s="39">
+        <v>0.42</v>
+      </c>
+      <c r="K31" s="52">
+        <f>ABS(J31-M31)</f>
+        <v>3.2999999999999696E-3</v>
+      </c>
+      <c r="L31" s="59"/>
+      <c r="M31" s="39">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="N31" s="52">
+        <f>ABS(M31-O31)</f>
+        <v>5.3299999999999959E-2</v>
+      </c>
+      <c r="O31" s="30">
+        <v>0.47</v>
+      </c>
+      <c r="P31" s="52">
+        <f>ABS(J31-O31)</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="39">
+        <v>0.41</v>
+      </c>
+      <c r="S31" s="52">
+        <f>ABS(R31-U31)</f>
+        <v>2.4999999999999967E-2</v>
+      </c>
+      <c r="U31" s="67">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="V31" s="52">
+        <f>ABS(U31-W31)</f>
+        <v>2.4999999999999967E-2</v>
+      </c>
+      <c r="W31" s="30">
+        <v>0.41</v>
+      </c>
+      <c r="X31" s="52">
+        <f>ABS(R31-W31)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="39">
-        <v>0.51</v>
-      </c>
-      <c r="F30" s="52">
-        <f>ABS(E30-G30)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="30">
-        <v>0.51</v>
-      </c>
-      <c r="H30" s="52">
-        <f>ABS(B30-G30)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="35"/>
-      <c r="J30" s="39">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="K30" s="52">
-        <f>ABS(J30-M30)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="N30" s="52">
-        <f>ABS(M30-O30)</f>
-        <v>1.9999999999999907E-2</v>
-      </c>
-      <c r="O30" s="39">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="P30" s="52">
-        <f>ABS(J30-O30)</f>
-        <v>1.9999999999999907E-2</v>
-      </c>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="39">
-        <v>0.66</v>
-      </c>
-      <c r="S30" s="52">
-        <f>ABS(R30-U30)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="T30" s="39"/>
-      <c r="U30" s="39">
-        <v>0.65</v>
-      </c>
-      <c r="V30" s="52">
-        <f>ABS(U30-W30)</f>
-        <v>0</v>
-      </c>
-      <c r="W30" s="30">
-        <v>0.65</v>
-      </c>
-      <c r="X30" s="52">
-        <f>ABS(R30-W30)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="35"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39"/>
-      <c r="X31" s="30"/>
     </row>
     <row r="32" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" s="39">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C32" s="52">
         <f>ABS(B32-E32)</f>
-        <v>4.0000000000000036E-3</v>
+        <v>1.8000000000000238E-3</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="39">
-        <v>0.22600000000000001</v>
+        <v>0.2918</v>
       </c>
       <c r="F32" s="52">
         <f>ABS(E32-G32)</f>
-        <v>4.4000000000000011E-2</v>
+        <v>0.12819999999999998</v>
       </c>
       <c r="G32" s="30">
-        <v>0.27</v>
+        <v>0.42</v>
       </c>
       <c r="H32" s="52">
         <f>ABS(B32-G32)</f>
-        <v>4.0000000000000008E-2</v>
+        <v>0.13</v>
       </c>
       <c r="I32" s="35"/>
       <c r="J32" s="39">
-        <v>0.42</v>
+        <v>0.32</v>
       </c>
       <c r="K32" s="52">
         <f>ABS(J32-M32)</f>
-        <v>3.2999999999999696E-3</v>
+        <v>1.2000000000000344E-3</v>
       </c>
       <c r="L32" s="59"/>
       <c r="M32" s="39">
-        <v>0.41670000000000001</v>
+        <v>0.31879999999999997</v>
       </c>
       <c r="N32" s="52">
         <f>ABS(M32-O32)</f>
-        <v>5.3299999999999959E-2</v>
+        <v>6.1200000000000032E-2</v>
       </c>
       <c r="O32" s="30">
-        <v>0.47</v>
+        <v>0.38</v>
       </c>
       <c r="P32" s="52">
         <f>ABS(J32-O32)</f>
-        <v>4.9999999999999989E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q32" s="35"/>
       <c r="R32" s="39">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="S32" s="52">
         <f>ABS(R32-U32)</f>
-        <v>2.4999999999999967E-2</v>
+        <v>1.319999999999999E-2</v>
       </c>
       <c r="U32" s="67">
-        <v>0.38500000000000001</v>
+        <v>0.33679999999999999</v>
       </c>
       <c r="V32" s="52">
         <f>ABS(U32-W32)</f>
-        <v>2.4999999999999967E-2</v>
+        <v>1.6799999999999982E-2</v>
       </c>
       <c r="W32" s="30">
-        <v>0.41</v>
+        <v>0.32</v>
       </c>
       <c r="X32" s="52">
         <f>ABS(R32-W32)</f>
-        <v>0</v>
+        <v>2.9999999999999971E-2</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" s="39">
-        <v>0.28999999999999998</v>
+        <v>0.64</v>
       </c>
       <c r="C33" s="52">
         <f>ABS(B33-E33)</f>
-        <v>1.8000000000000238E-3</v>
+        <v>9.099999999999997E-3</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" s="39">
-        <v>0.2918</v>
+        <v>0.64910000000000001</v>
       </c>
       <c r="F33" s="52">
         <f>ABS(E33-G33)</f>
-        <v>0.12819999999999998</v>
+        <v>0.18909999999999999</v>
       </c>
       <c r="G33" s="30">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="H33" s="52">
         <f>ABS(B33-G33)</f>
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="I33" s="35"/>
       <c r="J33" s="39">
-        <v>0.32</v>
+        <v>0.67</v>
       </c>
       <c r="K33" s="52">
         <f>ABS(J33-M33)</f>
-        <v>1.2000000000000344E-3</v>
+        <v>6.5999999999999392E-3</v>
       </c>
       <c r="L33" s="59"/>
       <c r="M33" s="39">
-        <v>0.31879999999999997</v>
+        <v>0.67659999999999998</v>
       </c>
       <c r="N33" s="52">
         <f>ABS(M33-O33)</f>
-        <v>6.1200000000000032E-2</v>
+        <v>0.33659999999999995</v>
       </c>
       <c r="O33" s="30">
-        <v>0.38</v>
+        <v>0.34</v>
       </c>
       <c r="P33" s="52">
         <f>ABS(J33-O33)</f>
-        <v>0.06</v>
+        <v>0.33</v>
       </c>
       <c r="Q33" s="35"/>
       <c r="R33" s="39">
-        <v>0.35</v>
+        <v>0.71</v>
       </c>
       <c r="S33" s="52">
         <f>ABS(R33-U33)</f>
-        <v>1.319999999999999E-2</v>
+        <v>1.4399999999999968E-2</v>
       </c>
       <c r="U33" s="67">
-        <v>0.33679999999999999</v>
+        <v>0.6956</v>
       </c>
       <c r="V33" s="52">
         <f>ABS(U33-W33)</f>
-        <v>1.6799999999999982E-2</v>
+        <v>4.3999999999999595E-3</v>
       </c>
       <c r="W33" s="30">
-        <v>0.32</v>
+        <v>0.7</v>
       </c>
       <c r="X33" s="52">
         <f>ABS(R33-W33)</f>
-        <v>2.9999999999999971E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="39">
-        <v>0.64</v>
-      </c>
-      <c r="C34" s="52">
-        <f>ABS(B34-E34)</f>
-        <v>9.099999999999997E-3</v>
-      </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="39">
-        <v>0.64910000000000001</v>
-      </c>
-      <c r="F34" s="52">
-        <f>ABS(E34-G34)</f>
-        <v>0.18909999999999999</v>
-      </c>
-      <c r="G34" s="30">
-        <v>0.46</v>
-      </c>
-      <c r="H34" s="52">
-        <f>ABS(B34-G34)</f>
-        <v>0.18</v>
-      </c>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
       <c r="I34" s="35"/>
-      <c r="J34" s="39">
-        <v>0.67</v>
-      </c>
-      <c r="K34" s="52">
-        <f>ABS(J34-M34)</f>
-        <v>6.5999999999999392E-3</v>
-      </c>
-      <c r="L34" s="59"/>
-      <c r="M34" s="39">
-        <v>0.67659999999999998</v>
-      </c>
-      <c r="N34" s="52">
-        <f>ABS(M34-O34)</f>
-        <v>0.33659999999999995</v>
-      </c>
-      <c r="O34" s="30">
-        <v>0.34</v>
-      </c>
-      <c r="P34" s="52">
-        <f>ABS(J34-O34)</f>
-        <v>0.33</v>
-      </c>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
       <c r="Q34" s="35"/>
-      <c r="R34" s="39">
-        <v>0.71</v>
-      </c>
-      <c r="S34" s="52">
-        <f>ABS(R34-U34)</f>
-        <v>1.4399999999999968E-2</v>
-      </c>
-      <c r="U34" s="67">
-        <v>0.6956</v>
-      </c>
-      <c r="V34" s="52">
-        <f>ABS(U34-W34)</f>
-        <v>4.3999999999999595E-3</v>
-      </c>
-      <c r="W34" s="30">
-        <v>0.7</v>
-      </c>
-      <c r="X34" s="52">
-        <f>ABS(R34-W34)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+      <c r="X34" s="30"/>
+    </row>
+    <row r="35" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="40">
+        <v>0</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
       <c r="E35" s="39"/>
@@ -5325,7 +5262,9 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
       <c r="I35" s="35"/>
-      <c r="J35" s="39"/>
+      <c r="J35" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="K35" s="39"/>
       <c r="L35" s="39"/>
       <c r="M35" s="39"/>
@@ -5333,15 +5272,32 @@
       <c r="O35" s="39"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="35"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-      <c r="X35" s="30"/>
+      <c r="R35" s="53">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="S35" s="52">
+        <f>ABS(R35-U35)</f>
+        <v>2.6999999999999941E-4</v>
+      </c>
+      <c r="T35" s="59"/>
+      <c r="U35" s="53">
+        <v>4.0730000000000002E-2</v>
+      </c>
+      <c r="V35" s="52">
+        <f>ABS(U35-W35)</f>
+        <v>5.2699999999999969E-3</v>
+      </c>
+      <c r="W35" s="30">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="X35" s="52">
+        <f>ABS(R35-W35)</f>
+        <v>4.9999999999999975E-3</v>
+      </c>
     </row>
     <row r="36" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B36" s="39" t="s">
         <v>68</v>
@@ -5364,31 +5320,31 @@
       <c r="P36" s="39"/>
       <c r="Q36" s="35"/>
       <c r="R36" s="53">
-        <v>4.1000000000000002E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="S36" s="52">
         <f>ABS(R36-U36)</f>
-        <v>2.6999999999999941E-4</v>
+        <v>3.0000000000000165E-4</v>
       </c>
       <c r="T36" s="59"/>
       <c r="U36" s="53">
-        <v>4.0730000000000002E-2</v>
+        <v>4.1700000000000001E-2</v>
       </c>
       <c r="V36" s="52">
         <f>ABS(U36-W36)</f>
-        <v>5.2699999999999969E-3</v>
+        <v>6.9999999999999923E-4</v>
       </c>
       <c r="W36" s="30">
-        <v>4.5999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="X36" s="52">
         <f>ABS(R36-W36)</f>
-        <v>4.9999999999999975E-3</v>
+        <v>1.0000000000000009E-3</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="39" t="s">
         <v>68</v>
@@ -5411,31 +5367,31 @@
       <c r="P37" s="39"/>
       <c r="Q37" s="35"/>
       <c r="R37" s="53">
-        <v>4.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="S37" s="52">
         <f>ABS(R37-U37)</f>
-        <v>3.0000000000000165E-4</v>
+        <v>2.9999999999999472E-4</v>
       </c>
       <c r="T37" s="59"/>
       <c r="U37" s="53">
-        <v>4.1700000000000001E-2</v>
+        <v>0.1017</v>
       </c>
       <c r="V37" s="52">
         <f>ABS(U37-W37)</f>
-        <v>6.9999999999999923E-4</v>
+        <v>1.2700000000000003E-2</v>
       </c>
       <c r="W37" s="30">
-        <v>4.1000000000000002E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="X37" s="52">
         <f>ABS(R37-W37)</f>
-        <v>1.0000000000000009E-3</v>
+        <v>1.2999999999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="40">
-        <v>2</v>
+      <c r="A38" s="40" t="s">
+        <v>69</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>68</v>
@@ -5458,45 +5414,41 @@
       <c r="P38" s="39"/>
       <c r="Q38" s="35"/>
       <c r="R38" s="53">
-        <v>0.10199999999999999</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="S38" s="52">
         <f>ABS(R38-U38)</f>
-        <v>2.9999999999999472E-4</v>
+        <v>4.1600000000002746E-4</v>
       </c>
       <c r="T38" s="59"/>
       <c r="U38" s="53">
-        <v>0.1017</v>
+        <v>0.285416</v>
       </c>
       <c r="V38" s="52">
         <f>ABS(U38-W38)</f>
-        <v>1.2700000000000003E-2</v>
+        <v>5.9415999999999997E-2</v>
       </c>
       <c r="W38" s="30">
-        <v>8.8999999999999996E-2</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="X38" s="52">
         <f>ABS(R38-W38)</f>
-        <v>1.2999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
+        <v>5.8999999999999969E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="38"/>
       <c r="I39" s="35"/>
-      <c r="J39" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="J39" s="39"/>
       <c r="K39" s="39"/>
       <c r="L39" s="39"/>
       <c r="M39" s="39"/>
@@ -5504,42 +5456,29 @@
       <c r="O39" s="39"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="35"/>
-      <c r="R39" s="53">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="S39" s="52">
-        <f>ABS(R39-U39)</f>
-        <v>4.1600000000002746E-4</v>
-      </c>
-      <c r="T39" s="59"/>
-      <c r="U39" s="53">
-        <v>0.285416</v>
-      </c>
-      <c r="V39" s="52">
-        <f>ABS(U39-W39)</f>
-        <v>5.9415999999999997E-2</v>
-      </c>
-      <c r="W39" s="30">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="X39" s="52">
-        <f>ABS(R39-W39)</f>
-        <v>5.8999999999999969E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="38"/>
+      <c r="R39" s="39"/>
+      <c r="S39" s="39"/>
+      <c r="T39" s="39"/>
+      <c r="U39" s="39"/>
+      <c r="X39" s="30"/>
+    </row>
+    <row r="40" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="35"/>
       <c r="I40" s="35"/>
-      <c r="J40" s="39"/>
+      <c r="J40" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="K40" s="39"/>
       <c r="L40" s="39"/>
       <c r="M40" s="39"/>
@@ -5547,15 +5486,32 @@
       <c r="O40" s="39"/>
       <c r="P40" s="39"/>
       <c r="Q40" s="35"/>
-      <c r="R40" s="39"/>
-      <c r="S40" s="39"/>
-      <c r="T40" s="39"/>
-      <c r="U40" s="39"/>
-      <c r="X40" s="30"/>
+      <c r="R40" s="53">
+        <v>0</v>
+      </c>
+      <c r="S40" s="52">
+        <f>ABS(R40-U40)</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="59"/>
+      <c r="U40" s="53">
+        <v>0</v>
+      </c>
+      <c r="V40" s="52">
+        <f>ABS(U40-W40)</f>
+        <v>0</v>
+      </c>
+      <c r="W40" s="30">
+        <v>0</v>
+      </c>
+      <c r="X40" s="52">
+        <f>ABS(R40-W40)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="39" t="s">
         <v>68</v>
@@ -5602,7 +5558,7 @@
     </row>
     <row r="42" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42" s="39" t="s">
         <v>68</v>
@@ -5625,22 +5581,22 @@
       <c r="P42" s="39"/>
       <c r="Q42" s="35"/>
       <c r="R42" s="53">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="S42" s="52">
         <f>ABS(R42-U42)</f>
-        <v>0</v>
+        <v>2.9999999999999992E-4</v>
       </c>
       <c r="T42" s="59"/>
       <c r="U42" s="53">
-        <v>0</v>
+        <v>1.37E-2</v>
       </c>
       <c r="V42" s="52">
         <f>ABS(U42-W42)</f>
-        <v>0</v>
+        <v>2.9999999999999992E-4</v>
       </c>
       <c r="W42" s="30">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="X42" s="52">
         <f>ABS(R42-W42)</f>
@@ -5649,7 +5605,7 @@
     </row>
     <row r="43" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B43" s="39" t="s">
         <v>68</v>
@@ -5672,22 +5628,22 @@
       <c r="P43" s="39"/>
       <c r="Q43" s="35"/>
       <c r="R43" s="53">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="S43" s="52">
         <f>ABS(R43-U43)</f>
-        <v>2.9999999999999992E-4</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="T43" s="59"/>
       <c r="U43" s="53">
-        <v>1.37E-2</v>
+        <v>3.6499999999999998E-2</v>
       </c>
       <c r="V43" s="52">
         <f>ABS(U43-W43)</f>
-        <v>2.9999999999999992E-4</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="W43" s="30">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="X43" s="52">
         <f>ABS(R43-W43)</f>
@@ -5696,7 +5652,7 @@
     </row>
     <row r="44" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="40" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B44" s="39" t="s">
         <v>68</v>
@@ -5719,22 +5675,22 @@
       <c r="P44" s="39"/>
       <c r="Q44" s="35"/>
       <c r="R44" s="53">
-        <v>3.6999999999999998E-2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="S44" s="52">
         <f>ABS(R44-U44)</f>
-        <v>5.0000000000000044E-4</v>
+        <v>3.2999999999999696E-4</v>
       </c>
       <c r="T44" s="59"/>
       <c r="U44" s="53">
-        <v>3.6499999999999998E-2</v>
+        <v>0.22467000000000001</v>
       </c>
       <c r="V44" s="52">
         <f>ABS(U44-W44)</f>
-        <v>5.0000000000000044E-4</v>
+        <v>3.2999999999999696E-4</v>
       </c>
       <c r="W44" s="30">
-        <v>3.6999999999999998E-2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="X44" s="52">
         <f>ABS(R44-W44)</f>
@@ -5742,22 +5698,18 @@
       </c>
     </row>
     <row r="45" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A45" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="39"/>
       <c r="C45" s="39"/>
       <c r="D45" s="39"/>
       <c r="E45" s="39"/>
-      <c r="F45" s="35"/>
+      <c r="F45" s="39"/>
       <c r="G45" s="39"/>
-      <c r="H45" s="35"/>
+      <c r="H45" s="39"/>
       <c r="I45" s="35"/>
-      <c r="J45" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="J45" s="39"/>
       <c r="K45" s="39"/>
       <c r="L45" s="39"/>
       <c r="M45" s="39"/>
@@ -5765,50 +5717,65 @@
       <c r="O45" s="39"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="35"/>
-      <c r="R45" s="53">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="S45" s="52">
-        <f>ABS(R45-U45)</f>
-        <v>3.2999999999999696E-4</v>
-      </c>
-      <c r="T45" s="59"/>
-      <c r="U45" s="53">
-        <v>0.22467000000000001</v>
-      </c>
-      <c r="V45" s="52">
-        <f>ABS(U45-W45)</f>
-        <v>3.2999999999999696E-4</v>
-      </c>
-      <c r="W45" s="30">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="X45" s="52">
-        <f>ABS(R45-W45)</f>
-        <v>0</v>
-      </c>
+      <c r="R45" s="39"/>
+      <c r="S45" s="39"/>
+      <c r="T45" s="39"/>
+      <c r="U45" s="39"/>
+      <c r="X45" s="30"/>
     </row>
     <row r="46" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
+      <c r="A46" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="57">
+        <v>122</v>
+      </c>
+      <c r="C46" s="52">
+        <f>ABS(B46-E46)</f>
+        <v>15.030000000000001</v>
+      </c>
+      <c r="D46" s="57"/>
+      <c r="E46" s="39">
+        <v>106.97</v>
+      </c>
+      <c r="F46" s="52">
+        <f>ABS(E46-G46)</f>
+        <v>36.72999999999999</v>
+      </c>
+      <c r="G46" s="30">
+        <v>143.69999999999999</v>
+      </c>
+      <c r="H46" s="52">
+        <f>ABS(B46-G46)</f>
+        <v>21.699999999999989</v>
+      </c>
       <c r="I46" s="35"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
+      <c r="J46" s="57">
+        <v>52.4</v>
+      </c>
+      <c r="K46" s="52">
+        <f>ABS(J46-M46)</f>
+        <v>6.9499999999999957</v>
+      </c>
+      <c r="L46" s="57"/>
+      <c r="M46" s="39">
+        <v>45.45</v>
+      </c>
+      <c r="N46" s="52">
+        <f>ABS(M46-O46)</f>
+        <v>21.849999999999994</v>
+      </c>
+      <c r="O46" s="30">
+        <v>67.3</v>
+      </c>
+      <c r="P46" s="52">
+        <f>ABS(J46-O46)</f>
+        <v>14.899999999999999</v>
+      </c>
       <c r="Q46" s="35"/>
-      <c r="R46" s="39"/>
+      <c r="R46" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="S46" s="39"/>
       <c r="T46" s="39"/>
       <c r="U46" s="39"/>
@@ -5816,52 +5783,52 @@
     </row>
     <row r="47" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="40" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B47" s="57">
-        <v>122</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="C47" s="52">
         <f>ABS(B47-E47)</f>
-        <v>15.030000000000001</v>
+        <v>7.1700000000000017</v>
       </c>
       <c r="D47" s="57"/>
       <c r="E47" s="39">
-        <v>106.97</v>
+        <v>42.97</v>
       </c>
       <c r="F47" s="52">
         <f>ABS(E47-G47)</f>
-        <v>36.72999999999999</v>
+        <v>11.530000000000001</v>
       </c>
       <c r="G47" s="30">
-        <v>143.69999999999999</v>
+        <v>54.5</v>
       </c>
       <c r="H47" s="52">
         <f>ABS(B47-G47)</f>
-        <v>21.699999999999989</v>
+        <v>18.700000000000003</v>
       </c>
       <c r="I47" s="35"/>
       <c r="J47" s="57">
-        <v>52.4</v>
+        <v>23.1</v>
       </c>
       <c r="K47" s="52">
         <f>ABS(J47-M47)</f>
-        <v>6.9499999999999957</v>
+        <v>8.2900000000000009</v>
       </c>
       <c r="L47" s="57"/>
       <c r="M47" s="39">
-        <v>45.45</v>
+        <v>14.81</v>
       </c>
       <c r="N47" s="52">
         <f>ABS(M47-O47)</f>
-        <v>21.849999999999994</v>
+        <v>29.79</v>
       </c>
       <c r="O47" s="30">
-        <v>67.3</v>
+        <v>44.6</v>
       </c>
       <c r="P47" s="52">
         <f>ABS(J47-O47)</f>
-        <v>14.899999999999999</v>
+        <v>21.5</v>
       </c>
       <c r="Q47" s="35"/>
       <c r="R47" s="39" t="s">
@@ -5874,188 +5841,153 @@
     </row>
     <row r="48" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="57">
-        <v>35.799999999999997</v>
+        <v>88.4</v>
       </c>
       <c r="C48" s="52">
         <f>ABS(B48-E48)</f>
-        <v>7.1700000000000017</v>
-      </c>
-      <c r="D48" s="57"/>
+        <v>4.3699999999999903</v>
+      </c>
+      <c r="D48" s="48"/>
       <c r="E48" s="39">
-        <v>42.97</v>
+        <v>92.77</v>
       </c>
       <c r="F48" s="52">
         <f>ABS(E48-G48)</f>
-        <v>11.530000000000001</v>
+        <v>4.3699999999999903</v>
       </c>
       <c r="G48" s="30">
-        <v>54.5</v>
+        <v>88.4</v>
       </c>
       <c r="H48" s="52">
         <f>ABS(B48-G48)</f>
-        <v>18.700000000000003</v>
+        <v>0</v>
       </c>
       <c r="I48" s="35"/>
       <c r="J48" s="57">
-        <v>23.1</v>
+        <v>49.7</v>
       </c>
       <c r="K48" s="52">
         <f>ABS(J48-M48)</f>
-        <v>8.2900000000000009</v>
+        <v>0.72999999999999687</v>
       </c>
       <c r="L48" s="57"/>
       <c r="M48" s="39">
-        <v>14.81</v>
+        <v>50.43</v>
       </c>
       <c r="N48" s="52">
         <f>ABS(M48-O48)</f>
-        <v>29.79</v>
+        <v>25.869999999999997</v>
       </c>
       <c r="O48" s="30">
-        <v>44.6</v>
+        <v>76.3</v>
       </c>
       <c r="P48" s="52">
         <f>ABS(J48-O48)</f>
-        <v>21.5</v>
+        <v>26.599999999999994</v>
       </c>
       <c r="Q48" s="35"/>
       <c r="R48" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="S48" s="39"/>
+      <c r="S48" s="35"/>
       <c r="T48" s="39"/>
       <c r="U48" s="39"/>
-      <c r="X48" s="30"/>
-    </row>
-    <row r="49" spans="1:24" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="57">
-        <v>88.4</v>
+    </row>
+    <row r="49" spans="1:24" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="71">
+        <v>256.60000000000002</v>
       </c>
       <c r="C49" s="52">
         <f>ABS(B49-E49)</f>
-        <v>4.3699999999999903</v>
-      </c>
-      <c r="D49" s="48"/>
-      <c r="E49" s="39">
-        <v>92.77</v>
+        <v>75.510000000000019</v>
+      </c>
+      <c r="D49" s="49"/>
+      <c r="E49" s="65">
+        <v>181.09</v>
       </c>
       <c r="F49" s="52">
         <f>ABS(E49-G49)</f>
-        <v>4.3699999999999903</v>
-      </c>
-      <c r="G49" s="30">
-        <v>88.4</v>
+        <v>7.6099999999999852</v>
+      </c>
+      <c r="G49" s="69">
+        <v>188.7</v>
       </c>
       <c r="H49" s="52">
         <f>ABS(B49-G49)</f>
-        <v>0</v>
-      </c>
-      <c r="I49" s="35"/>
-      <c r="J49" s="57">
-        <v>49.7</v>
+        <v>67.900000000000034</v>
+      </c>
+      <c r="I49" s="42"/>
+      <c r="J49" s="71">
+        <v>59.1</v>
       </c>
       <c r="K49" s="52">
         <f>ABS(J49-M49)</f>
-        <v>0.72999999999999687</v>
-      </c>
-      <c r="L49" s="57"/>
-      <c r="M49" s="39">
-        <v>50.43</v>
+        <v>2.0500000000000043</v>
+      </c>
+      <c r="L49" s="49"/>
+      <c r="M49" s="65">
+        <v>57.05</v>
       </c>
       <c r="N49" s="52">
         <f>ABS(M49-O49)</f>
-        <v>25.869999999999997</v>
-      </c>
-      <c r="O49" s="30">
-        <v>76.3</v>
+        <v>24.549999999999997</v>
+      </c>
+      <c r="O49" s="69">
+        <v>81.599999999999994</v>
       </c>
       <c r="P49" s="52">
         <f>ABS(J49-O49)</f>
-        <v>26.599999999999994</v>
-      </c>
-      <c r="Q49" s="35"/>
-      <c r="R49" s="39" t="s">
+        <v>22.499999999999993</v>
+      </c>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="S49" s="35"/>
-      <c r="T49" s="39"/>
-      <c r="U49" s="39"/>
-    </row>
-    <row r="50" spans="1:24" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" s="71">
-        <v>256.60000000000002</v>
-      </c>
-      <c r="C50" s="52">
-        <f>ABS(B50-E50)</f>
-        <v>75.510000000000019</v>
-      </c>
-      <c r="D50" s="49"/>
-      <c r="E50" s="65">
-        <v>181.09</v>
-      </c>
-      <c r="F50" s="52">
-        <f>ABS(E50-G50)</f>
-        <v>7.6099999999999852</v>
-      </c>
-      <c r="G50" s="69">
-        <v>188.7</v>
-      </c>
-      <c r="H50" s="52">
-        <f>ABS(B50-G50)</f>
-        <v>67.900000000000034</v>
-      </c>
-      <c r="I50" s="42"/>
-      <c r="J50" s="71">
-        <v>59.1</v>
-      </c>
-      <c r="K50" s="52">
-        <f>ABS(J50-M50)</f>
-        <v>2.0500000000000043</v>
-      </c>
-      <c r="L50" s="49"/>
-      <c r="M50" s="65">
-        <v>57.05</v>
-      </c>
-      <c r="N50" s="52">
-        <f>ABS(M50-O50)</f>
-        <v>24.549999999999997</v>
-      </c>
-      <c r="O50" s="69">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="P50" s="52">
-        <f>ABS(J50-O50)</f>
-        <v>22.499999999999993</v>
-      </c>
-      <c r="Q50" s="42"/>
-      <c r="R50" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="S50" s="42"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="65"/>
-      <c r="V50" s="51"/>
-      <c r="W50" s="69"/>
-      <c r="X50" s="51"/>
-    </row>
-    <row r="51" spans="1:24" ht="13" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="41"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="41"/>
+      <c r="S49" s="42"/>
+      <c r="T49" s="42"/>
+      <c r="U49" s="65"/>
+      <c r="V49" s="51"/>
+      <c r="W49" s="69"/>
+      <c r="X49" s="51"/>
+    </row>
+    <row r="50" spans="1:24" ht="13" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="41"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="66"/>
+      <c r="P50" s="41"/>
+      <c r="Q50" s="41"/>
+      <c r="R50" s="66"/>
+      <c r="S50" s="41"/>
+      <c r="T50" s="41"/>
+      <c r="U50" s="66"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A51" s="43"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
       <c r="I51" s="41"/>
       <c r="J51" s="66"/>
       <c r="K51" s="41"/>
@@ -6139,15 +6071,15 @@
       <c r="T54" s="41"/>
       <c r="U54" s="66"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A55" s="43"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
+    <row r="55" spans="1:24" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
       <c r="I55" s="41"/>
       <c r="J55" s="66"/>
       <c r="K55" s="41"/>
@@ -6162,15 +6094,15 @@
       <c r="T55" s="41"/>
       <c r="U55" s="66"/>
     </row>
-    <row r="56" spans="1:24" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="44"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
       <c r="I56" s="41"/>
       <c r="J56" s="66"/>
       <c r="K56" s="41"/>
@@ -6185,42 +6117,19 @@
       <c r="T56" s="41"/>
       <c r="U56" s="66"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="66"/>
-      <c r="K57" s="41"/>
-      <c r="L57" s="41"/>
-      <c r="M57" s="66"/>
-      <c r="N57" s="41"/>
-      <c r="O57" s="66"/>
-      <c r="P57" s="41"/>
-      <c r="Q57" s="41"/>
-      <c r="R57" s="66"/>
-      <c r="S57" s="41"/>
-      <c r="T57" s="41"/>
-      <c r="U57" s="66"/>
-    </row>
-    <row r="59" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="27"/>
-    </row>
-    <row r="61" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="27"/>
+    <row r="58" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="27"/>
+    </row>
+    <row r="60" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C34">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="C5:C33">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6229,8 +6138,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F34">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="F5:F33">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6239,8 +6148,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H34">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="H5:H33">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6249,8 +6158,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K34">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="K5:K33">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6259,8 +6168,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N34">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="N5:N33">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6269,8 +6178,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P5:P34">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="P5:P33">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6279,8 +6188,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5:S34">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="S5:S33">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6289,8 +6198,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V34">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="V5:V33">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6299,8 +6208,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X5:X34">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="X5:X33">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>